<commit_message>
delete file not used
</commit_message>
<xml_diff>
--- a/Hasil_Pengujian_Map_2_128.xlsx
+++ b/Hasil_Pengujian_Map_2_128.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMHAS\TA_Python_Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E85B186-D255-4857-8D00-AB186F44BD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE20BF5-0964-4A0A-BE4C-6D8CA6EE475D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="6120" windowWidth="11712" windowHeight="6216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Waktu Pencarian" sheetId="1" r:id="rId1"/>
@@ -698,7 +698,7 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="A1:F97"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,222 +728,222 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>1.7000000000000001E-4</v>
+        <v>9.5549999999999997E-4</v>
       </c>
       <c r="D2">
-        <v>4.44E-4</v>
+        <v>2.5665000000000002E-3</v>
       </c>
       <c r="E2">
-        <v>9.7999999999999997E-4</v>
+        <v>1.6927500000000002E-2</v>
       </c>
       <c r="F2">
-        <v>2.0509999999999999E-3</v>
+        <v>0.11158949999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>2.3000000000000001E-4</v>
+        <v>2.4399999999999999E-4</v>
       </c>
       <c r="D3">
-        <v>4.6000000000000001E-4</v>
+        <v>1.0610000000000001E-3</v>
       </c>
       <c r="E3">
-        <v>1.1039999999999999E-3</v>
+        <v>4.6540000000000002E-3</v>
       </c>
       <c r="F3">
-        <v>2.1570000000000001E-3</v>
+        <v>1.8636E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>2.1900000000000001E-4</v>
+        <v>4.5199999999999998E-4</v>
       </c>
       <c r="D4">
-        <v>5.5099999999999995E-4</v>
+        <v>1.379E-3</v>
       </c>
       <c r="E4">
-        <v>1.2819999999999999E-3</v>
+        <v>5.1905000000000007E-3</v>
       </c>
       <c r="F4">
-        <v>2.4299999999999999E-3</v>
+        <v>2.1794999999999998E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>1.4999999999999999E-4</v>
+        <v>9.3749999999999997E-4</v>
       </c>
       <c r="D5">
-        <v>5.4500000000000002E-4</v>
+        <v>1.7485000000000001E-3</v>
       </c>
       <c r="E5">
-        <v>1.467E-3</v>
+        <v>9.5079999999999991E-3</v>
       </c>
       <c r="F5">
-        <v>2.8050000000000002E-3</v>
+        <v>6.8498000000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>2.41E-4</v>
+        <v>4.46E-4</v>
       </c>
       <c r="D6">
-        <v>5.53E-4</v>
+        <v>2.0225E-3</v>
       </c>
       <c r="E6">
-        <v>1.4580000000000001E-3</v>
+        <v>1.3827000000000001E-2</v>
       </c>
       <c r="F6">
-        <v>3.0639999999999999E-3</v>
+        <v>9.0217999999999993E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>2.2900000000000001E-4</v>
+        <v>1.0839999999999999E-3</v>
       </c>
       <c r="D7">
-        <v>5.7300000000000005E-4</v>
+        <v>2.4784999999999998E-3</v>
       </c>
       <c r="E7">
-        <v>1.361E-3</v>
+        <v>1.50565E-2</v>
       </c>
       <c r="F7">
-        <v>3.3159999999999999E-3</v>
+        <v>0.100032</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>2.6699999999999998E-4</v>
+        <v>1.1410000000000001E-3</v>
       </c>
       <c r="D8">
-        <v>7.0200000000000004E-4</v>
+        <v>2.6424999999999999E-3</v>
       </c>
       <c r="E8">
-        <v>2.8679999999999999E-3</v>
+        <v>1.7187999999999998E-2</v>
       </c>
       <c r="F8">
-        <v>3.3730000000000001E-3</v>
+        <v>0.1120165</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>2.1000000000000001E-4</v>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="D9">
-        <v>6.6399999999999999E-4</v>
+        <v>5.4500000000000002E-4</v>
       </c>
       <c r="E9">
-        <v>1.755E-3</v>
+        <v>1.467E-3</v>
       </c>
       <c r="F9">
-        <v>3.8920000000000001E-3</v>
+        <v>2.8050000000000002E-3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>3.2699999999999998E-4</v>
+        <v>3.77E-4</v>
       </c>
       <c r="D10">
-        <v>1.096E-3</v>
+        <v>7.2599999999999997E-4</v>
       </c>
       <c r="E10">
-        <v>2.712E-3</v>
+        <v>2.0899999999999998E-3</v>
       </c>
       <c r="F10">
-        <v>7.2370000000000004E-3</v>
+        <v>7.9014999999999988E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>2.31E-4</v>
+        <v>3.8949999999999998E-4</v>
       </c>
       <c r="D11">
-        <v>5.8500000000000002E-4</v>
+        <v>1.4965E-3</v>
       </c>
       <c r="E11">
-        <v>2.0509999999999999E-3</v>
+        <v>4.1150000000000006E-3</v>
       </c>
       <c r="F11">
-        <v>7.6660000000000001E-3</v>
+        <v>1.4791E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="C12">
-        <v>4.0299999999999998E-4</v>
+        <v>3.1E-4</v>
       </c>
       <c r="D12">
-        <v>1.3090000000000001E-3</v>
+        <v>9.7400000000000004E-4</v>
       </c>
       <c r="E12">
-        <v>2.931E-3</v>
+        <v>4.1469999999999996E-3</v>
       </c>
       <c r="F12">
-        <v>7.816E-3</v>
+        <v>1.6278000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -951,239 +951,239 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>3.77E-4</v>
+        <v>2.1699999999999999E-4</v>
       </c>
       <c r="D13">
-        <v>7.2599999999999997E-4</v>
+        <v>9.0700000000000004E-4</v>
       </c>
       <c r="E13">
-        <v>2.0899999999999998E-3</v>
+        <v>4.1460000000000004E-3</v>
       </c>
       <c r="F13">
-        <v>7.9014999999999988E-3</v>
+        <v>1.8234E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>3.4600000000000001E-4</v>
+        <v>2.8800000000000001E-4</v>
       </c>
       <c r="D14">
-        <v>1.116E-3</v>
+        <v>1.1460000000000001E-3</v>
       </c>
       <c r="E14">
-        <v>2.9020000000000001E-3</v>
+        <v>4.6820000000000004E-3</v>
       </c>
       <c r="F14">
-        <v>7.9900000000000006E-3</v>
+        <v>1.8748999999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>3.8249999999999997E-4</v>
+        <v>2.7399999999999999E-4</v>
       </c>
       <c r="D15">
-        <v>7.4600000000000003E-4</v>
+        <v>1.077E-3</v>
       </c>
       <c r="E15">
-        <v>2.0325E-3</v>
+        <v>4.5100000000000001E-3</v>
       </c>
       <c r="F15">
-        <v>8.0255000000000014E-3</v>
+        <v>1.9091E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C16">
-        <v>4.64E-4</v>
+        <v>4.6099999999999998E-4</v>
       </c>
       <c r="D16">
-        <v>7.7050000000000003E-4</v>
+        <v>1.4189999999999999E-3</v>
       </c>
       <c r="E16">
-        <v>2.1050000000000001E-3</v>
+        <v>4.9179999999999996E-3</v>
       </c>
       <c r="F16">
-        <v>8.0464999999999998E-3</v>
+        <v>2.0695000000000002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="C17">
-        <v>2.6899999999999998E-4</v>
+        <v>5.1749999999999995E-4</v>
       </c>
       <c r="D17">
-        <v>6.5099999999999999E-4</v>
+        <v>1.4235000000000001E-3</v>
       </c>
       <c r="E17">
-        <v>2.147E-3</v>
+        <v>5.2325000000000002E-3</v>
       </c>
       <c r="F17">
-        <v>8.1060000000000004E-3</v>
+        <v>2.17755E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C18">
-        <v>4.0650000000000001E-4</v>
+        <v>3.4699999999999998E-4</v>
       </c>
       <c r="D18">
-        <v>8.1149999999999994E-4</v>
+        <v>1.3359999999999999E-3</v>
       </c>
       <c r="E18">
-        <v>2.1445000000000001E-3</v>
+        <v>4.9909999999999998E-3</v>
       </c>
       <c r="F18">
-        <v>8.2389999999999998E-3</v>
+        <v>2.2544000000000002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="C19">
-        <v>2.9E-4</v>
+        <v>1.1225E-3</v>
       </c>
       <c r="D19">
-        <v>8.4599999999999996E-4</v>
+        <v>1.7930000000000001E-3</v>
       </c>
       <c r="E19">
-        <v>2.379E-3</v>
+        <v>9.3880000000000005E-3</v>
       </c>
       <c r="F19">
-        <v>8.4690000000000008E-3</v>
+        <v>6.8598999999999993E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="C20">
-        <v>3.1799999999999998E-4</v>
+        <v>5.1350000000000007E-4</v>
       </c>
       <c r="D20">
-        <v>8.5400000000000005E-4</v>
+        <v>2.006E-3</v>
       </c>
       <c r="E20">
-        <v>2.5070000000000001E-3</v>
+        <v>1.1375E-2</v>
       </c>
       <c r="F20">
-        <v>8.6029999999999995E-3</v>
+        <v>6.9242999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="C21">
-        <v>3.9899999999999999E-4</v>
+        <v>5.0850000000000005E-4</v>
       </c>
       <c r="D21">
-        <v>1.201E-3</v>
+        <v>2.1105E-3</v>
       </c>
       <c r="E21">
-        <v>3.1749999999999999E-3</v>
+        <v>1.4120000000000001E-2</v>
       </c>
       <c r="F21">
-        <v>8.8240000000000002E-3</v>
+        <v>9.1477500000000003E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C22">
-        <v>3.2200000000000002E-4</v>
+        <v>5.7649999999999997E-4</v>
       </c>
       <c r="D22">
-        <v>9.5100000000000002E-4</v>
+        <v>2.1580000000000002E-3</v>
       </c>
       <c r="E22">
-        <v>2.5890000000000002E-3</v>
+        <v>1.3648E-2</v>
       </c>
       <c r="F22">
-        <v>9.3810000000000004E-3</v>
+        <v>9.7140499999999991E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C23">
-        <v>3.6699999999999998E-4</v>
+        <v>7.5700000000000008E-4</v>
       </c>
       <c r="D23">
-        <v>8.12E-4</v>
+        <v>2.3995000000000002E-3</v>
       </c>
       <c r="E23">
-        <v>2.447E-3</v>
+        <v>1.074E-2</v>
       </c>
       <c r="F23">
-        <v>9.7380000000000001E-3</v>
+        <v>9.7824500000000009E-2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C24">
-        <v>3.9599999999999998E-4</v>
+        <v>1.2784999999999999E-3</v>
       </c>
       <c r="D24">
-        <v>8.6700000000000004E-4</v>
+        <v>2.5214999999999999E-3</v>
       </c>
       <c r="E24">
-        <v>2.5469999999999998E-3</v>
+        <v>1.5318999999999999E-2</v>
       </c>
       <c r="F24">
-        <v>1.0356000000000001E-2</v>
+        <v>0.1004125</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1191,99 +1191,99 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C25">
-        <v>4.3300000000000001E-4</v>
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="D25">
-        <v>9.8700000000000003E-4</v>
+        <v>4.44E-4</v>
       </c>
       <c r="E25">
-        <v>2.8210000000000002E-3</v>
+        <v>9.7999999999999997E-4</v>
       </c>
       <c r="F25">
-        <v>1.05565E-2</v>
+        <v>2.0509999999999999E-3</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C26">
-        <v>3.7149999999999998E-4</v>
+        <v>2.3000000000000001E-4</v>
       </c>
       <c r="D26">
-        <v>9.7199999999999999E-4</v>
+        <v>4.6000000000000001E-4</v>
       </c>
       <c r="E26">
-        <v>2.7994999999999999E-3</v>
+        <v>1.1039999999999999E-3</v>
       </c>
       <c r="F26">
-        <v>1.05755E-2</v>
+        <v>2.1570000000000001E-3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="C27">
-        <v>4.26E-4</v>
+        <v>2.1000000000000001E-4</v>
       </c>
       <c r="D27">
-        <v>1.0560000000000001E-3</v>
+        <v>6.6399999999999999E-4</v>
       </c>
       <c r="E27">
-        <v>2.8530000000000001E-3</v>
+        <v>1.755E-3</v>
       </c>
       <c r="F27">
-        <v>1.07435E-2</v>
+        <v>3.8920000000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C28">
-        <v>4.2949999999999998E-4</v>
+        <v>2.31E-4</v>
       </c>
       <c r="D28">
-        <v>1.0675000000000001E-3</v>
+        <v>5.8500000000000002E-4</v>
       </c>
       <c r="E28">
-        <v>2.8465000000000001E-3</v>
+        <v>2.0509999999999999E-3</v>
       </c>
       <c r="F28">
-        <v>1.0792E-2</v>
+        <v>7.6660000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="C29">
-        <v>3.8099999999999999E-4</v>
+        <v>3.8249999999999997E-4</v>
       </c>
       <c r="D29">
-        <v>1.052E-3</v>
+        <v>7.4600000000000003E-4</v>
       </c>
       <c r="E29">
-        <v>3.2699999999999999E-3</v>
+        <v>2.0325E-3</v>
       </c>
       <c r="F29">
-        <v>1.0926E-2</v>
+        <v>8.0255000000000014E-3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1291,79 +1291,79 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C30">
-        <v>2.7300000000000002E-4</v>
+        <v>4.0650000000000001E-4</v>
       </c>
       <c r="D30">
-        <v>9.0200000000000002E-4</v>
+        <v>8.1149999999999994E-4</v>
       </c>
       <c r="E30">
-        <v>2.7810000000000001E-3</v>
+        <v>2.1445000000000001E-3</v>
       </c>
       <c r="F30">
-        <v>1.0972000000000001E-2</v>
+        <v>8.2389999999999998E-3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="C31">
-        <v>3.2400000000000001E-4</v>
+        <v>3.6699999999999998E-4</v>
       </c>
       <c r="D31">
-        <v>9.5699999999999995E-4</v>
+        <v>8.12E-4</v>
       </c>
       <c r="E31">
-        <v>3.0839999999999999E-3</v>
+        <v>2.447E-3</v>
       </c>
       <c r="F31">
-        <v>1.1233999999999999E-2</v>
+        <v>9.7380000000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C32">
-        <v>3.3700000000000001E-4</v>
+        <v>4.3300000000000001E-4</v>
       </c>
       <c r="D32">
-        <v>9.8900000000000008E-4</v>
+        <v>9.8700000000000003E-4</v>
       </c>
       <c r="E32">
-        <v>3.0240000000000002E-3</v>
+        <v>2.8210000000000002E-3</v>
       </c>
       <c r="F32">
-        <v>1.1409000000000001E-2</v>
+        <v>1.05565E-2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="C33">
-        <v>2.8600000000000001E-4</v>
+        <v>2.7300000000000002E-4</v>
       </c>
       <c r="D33">
-        <v>9.2299999999999999E-4</v>
+        <v>9.0200000000000002E-4</v>
       </c>
       <c r="E33">
-        <v>3.0040000000000002E-3</v>
+        <v>2.7810000000000001E-3</v>
       </c>
       <c r="F33">
-        <v>1.149E-2</v>
+        <v>1.0972000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1388,322 +1388,322 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="C35">
-        <v>2.2599999999999999E-4</v>
+        <v>3.59E-4</v>
       </c>
       <c r="D35">
-        <v>8.5700000000000001E-4</v>
+        <v>8.9400000000000005E-4</v>
       </c>
       <c r="E35">
-        <v>3.2179999999999999E-3</v>
+        <v>3.4529999999999999E-3</v>
       </c>
       <c r="F35">
-        <v>1.1612000000000001E-2</v>
+        <v>1.3957000000000001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="C36">
-        <v>2.6600000000000001E-4</v>
+        <v>4.26E-4</v>
       </c>
       <c r="D36">
-        <v>9.0499999999999999E-4</v>
+        <v>1.3205000000000001E-3</v>
       </c>
       <c r="E36">
-        <v>3.212E-3</v>
+        <v>4.1805000000000002E-3</v>
       </c>
       <c r="F36">
-        <v>1.1629E-2</v>
+        <v>1.48775E-2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C37">
-        <v>3.79E-4</v>
+        <v>3.9550000000000002E-4</v>
       </c>
       <c r="D37">
-        <v>1.0399999999999999E-3</v>
+        <v>1.2899999999999999E-3</v>
       </c>
       <c r="E37">
-        <v>3.5040000000000002E-3</v>
+        <v>4.1330000000000004E-3</v>
       </c>
       <c r="F37">
-        <v>1.1759E-2</v>
+        <v>1.5158E-2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="C38">
-        <v>3.9300000000000001E-4</v>
+        <v>3.6499999999999998E-4</v>
       </c>
       <c r="D38">
-        <v>1.1980000000000001E-3</v>
+        <v>1.0380000000000001E-3</v>
       </c>
       <c r="E38">
-        <v>3.2780000000000001E-3</v>
+        <v>4.3949999999999996E-3</v>
       </c>
       <c r="F38">
-        <v>1.1771E-2</v>
+        <v>1.6303000000000002E-2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C39">
-        <v>3.6299999999999999E-4</v>
+        <v>2.6200000000000003E-4</v>
       </c>
       <c r="D39">
-        <v>1.15E-3</v>
+        <v>9.5299999999999996E-4</v>
       </c>
       <c r="E39">
-        <v>3.2030000000000001E-3</v>
+        <v>4.2750000000000002E-3</v>
       </c>
       <c r="F39">
-        <v>1.1877E-2</v>
+        <v>1.8179000000000001E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="C40">
-        <v>4.1199999999999999E-4</v>
+        <v>2.7999999999999998E-4</v>
       </c>
       <c r="D40">
-        <v>1.1360000000000001E-3</v>
+        <v>1.023E-3</v>
       </c>
       <c r="E40">
-        <v>3.5720000000000001E-3</v>
+        <v>4.3489999999999996E-3</v>
       </c>
       <c r="F40">
-        <v>1.2093E-2</v>
+        <v>1.9205E-2</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="C41">
-        <v>3.5799999999999997E-4</v>
+        <v>3.19E-4</v>
       </c>
       <c r="D41">
-        <v>1.0349999999999999E-3</v>
+        <v>1.2099999999999999E-3</v>
       </c>
       <c r="E41">
-        <v>2.4229999999999998E-3</v>
+        <v>4.6680000000000003E-3</v>
       </c>
       <c r="F41">
-        <v>1.2233000000000001E-2</v>
+        <v>1.9258999999999998E-2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42">
-        <v>3.6900000000000002E-4</v>
+        <v>4.9649999999999998E-4</v>
       </c>
       <c r="D42">
-        <v>1.4989999999999999E-3</v>
+        <v>1.4265E-3</v>
       </c>
       <c r="E42">
-        <v>3.6830000000000001E-3</v>
+        <v>4.9754999999999999E-3</v>
       </c>
       <c r="F42">
-        <v>1.2311000000000001E-2</v>
+        <v>2.0997999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="C43">
-        <v>4.0000000000000002E-4</v>
+        <v>3.9199999999999999E-4</v>
       </c>
       <c r="D43">
-        <v>1.142E-3</v>
+        <v>1.3849999999999999E-3</v>
       </c>
       <c r="E43">
-        <v>2.421E-3</v>
+        <v>5.2180000000000004E-3</v>
       </c>
       <c r="F43">
-        <v>1.2428E-2</v>
+        <v>2.3460999999999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="C44">
-        <v>2.31E-4</v>
+        <v>3.8699999999999997E-4</v>
       </c>
       <c r="D44">
-        <v>9.41E-4</v>
+        <v>1.5319999999999999E-3</v>
       </c>
       <c r="E44">
-        <v>2.5690000000000001E-3</v>
+        <v>6.1859999999999997E-3</v>
       </c>
       <c r="F44">
-        <v>1.3143E-2</v>
+        <v>3.0535E-2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>32</v>
       </c>
       <c r="C45">
-        <v>2.9100000000000003E-4</v>
+        <v>3.7399999999999998E-4</v>
       </c>
       <c r="D45">
-        <v>1.157E-3</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E45">
-        <v>3.718E-3</v>
+        <v>7.9869999999999993E-3</v>
       </c>
       <c r="F45">
-        <v>1.3157E-2</v>
+        <v>3.9775999999999999E-2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="C46">
-        <v>3.9599999999999998E-4</v>
+        <v>5.8399999999999999E-4</v>
       </c>
       <c r="D46">
-        <v>1.209E-3</v>
+        <v>2.0704999999999999E-3</v>
       </c>
       <c r="E46">
-        <v>3.803E-3</v>
+        <v>1.14365E-2</v>
       </c>
       <c r="F46">
-        <v>1.3332E-2</v>
+        <v>6.9770499999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="C47">
-        <v>2.7900000000000001E-4</v>
+        <v>5.3000000000000009E-4</v>
       </c>
       <c r="D47">
-        <v>1.0200000000000001E-3</v>
+        <v>2.0045000000000002E-3</v>
       </c>
       <c r="E47">
-        <v>2.65E-3</v>
+        <v>1.1518499999999999E-2</v>
       </c>
       <c r="F47">
-        <v>1.3396999999999999E-2</v>
+        <v>7.0735500000000007E-2</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="C48">
-        <v>2.4000000000000001E-4</v>
+        <v>4.5600000000000003E-4</v>
       </c>
       <c r="D48">
-        <v>8.2299999999999995E-4</v>
+        <v>2.2285E-3</v>
       </c>
       <c r="E48">
-        <v>3.1480000000000002E-3</v>
+        <v>1.392E-2</v>
       </c>
       <c r="F48">
-        <v>1.3505E-2</v>
+        <v>8.5014499999999993E-2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
       <c r="C49">
-        <v>2.7599999999999999E-4</v>
+        <v>6.4400000000000004E-4</v>
       </c>
       <c r="D49">
-        <v>8.9099999999999997E-4</v>
+        <v>2.493E-3</v>
       </c>
       <c r="E49">
-        <v>3.2330000000000002E-3</v>
+        <v>1.1592E-2</v>
       </c>
       <c r="F49">
-        <v>1.3602E-2</v>
+        <v>9.8580500000000001E-2</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C50">
-        <v>3.59E-4</v>
+        <v>2.1900000000000001E-4</v>
       </c>
       <c r="D50">
-        <v>8.9400000000000005E-4</v>
+        <v>5.5099999999999995E-4</v>
       </c>
       <c r="E50">
-        <v>3.4529999999999999E-3</v>
+        <v>1.2819999999999999E-3</v>
       </c>
       <c r="F50">
-        <v>1.3957000000000001E-2</v>
+        <v>2.4299999999999999E-3</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1711,79 +1711,79 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C51">
-        <v>4.0499999999999998E-4</v>
+        <v>2.41E-4</v>
       </c>
       <c r="D51">
-        <v>9.7099999999999997E-4</v>
+        <v>5.53E-4</v>
       </c>
       <c r="E51">
-        <v>3.473E-3</v>
+        <v>1.4580000000000001E-3</v>
       </c>
       <c r="F51">
-        <v>1.4128E-2</v>
+        <v>3.0639999999999999E-3</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C52">
-        <v>3.8949999999999998E-4</v>
+        <v>2.2900000000000001E-4</v>
       </c>
       <c r="D52">
-        <v>1.4965E-3</v>
+        <v>5.7300000000000005E-4</v>
       </c>
       <c r="E52">
-        <v>4.1150000000000006E-3</v>
+        <v>1.361E-3</v>
       </c>
       <c r="F52">
-        <v>1.4791E-2</v>
+        <v>3.3159999999999999E-3</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C53">
-        <v>4.26E-4</v>
+        <v>3.2699999999999998E-4</v>
       </c>
       <c r="D53">
-        <v>1.3205000000000001E-3</v>
+        <v>1.096E-3</v>
       </c>
       <c r="E53">
-        <v>4.1805000000000002E-3</v>
+        <v>2.712E-3</v>
       </c>
       <c r="F53">
-        <v>1.48775E-2</v>
+        <v>7.2370000000000004E-3</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="C54">
-        <v>3.9550000000000002E-4</v>
+        <v>4.64E-4</v>
       </c>
       <c r="D54">
-        <v>1.2899999999999999E-3</v>
+        <v>7.7050000000000003E-4</v>
       </c>
       <c r="E54">
-        <v>4.1330000000000004E-3</v>
+        <v>2.1050000000000001E-3</v>
       </c>
       <c r="F54">
-        <v>1.5158E-2</v>
+        <v>8.0464999999999998E-3</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1791,59 +1791,59 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C55">
-        <v>4.4749999999999998E-4</v>
+        <v>2.6899999999999998E-4</v>
       </c>
       <c r="D55">
-        <v>1.3324999999999999E-3</v>
+        <v>6.5099999999999999E-4</v>
       </c>
       <c r="E55">
-        <v>4.28E-3</v>
+        <v>2.147E-3</v>
       </c>
       <c r="F55">
-        <v>1.5374000000000001E-2</v>
+        <v>8.1060000000000004E-3</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="C56">
-        <v>3.1E-4</v>
+        <v>2.9E-4</v>
       </c>
       <c r="D56">
-        <v>9.7400000000000004E-4</v>
+        <v>8.4599999999999996E-4</v>
       </c>
       <c r="E56">
-        <v>4.1469999999999996E-3</v>
+        <v>2.379E-3</v>
       </c>
       <c r="F56">
-        <v>1.6278000000000001E-2</v>
+        <v>8.4690000000000008E-3</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C57">
-        <v>3.6499999999999998E-4</v>
+        <v>3.2200000000000002E-4</v>
       </c>
       <c r="D57">
-        <v>1.0380000000000001E-3</v>
+        <v>9.5100000000000002E-4</v>
       </c>
       <c r="E57">
-        <v>4.3949999999999996E-3</v>
+        <v>2.5890000000000002E-3</v>
       </c>
       <c r="F57">
-        <v>1.6303000000000002E-2</v>
+        <v>9.3810000000000004E-3</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1851,159 +1851,159 @@
         <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C58">
-        <v>3.5100000000000002E-4</v>
+        <v>3.9599999999999998E-4</v>
       </c>
       <c r="D58">
-        <v>9.7599999999999998E-4</v>
+        <v>8.6700000000000004E-4</v>
       </c>
       <c r="E58">
-        <v>3.6240000000000001E-3</v>
+        <v>2.5469999999999998E-3</v>
       </c>
       <c r="F58">
-        <v>1.7665E-2</v>
+        <v>1.0356000000000001E-2</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C59">
-        <v>3.79E-4</v>
+        <v>3.7149999999999998E-4</v>
       </c>
       <c r="D59">
-        <v>9.8799999999999995E-4</v>
+        <v>9.7199999999999999E-4</v>
       </c>
       <c r="E59">
-        <v>3.6960000000000001E-3</v>
+        <v>2.7994999999999999E-3</v>
       </c>
       <c r="F59">
-        <v>1.7812000000000001E-2</v>
+        <v>1.05755E-2</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C60">
-        <v>3.57E-4</v>
+        <v>4.2949999999999998E-4</v>
       </c>
       <c r="D60">
-        <v>1.085E-3</v>
+        <v>1.0675000000000001E-3</v>
       </c>
       <c r="E60">
-        <v>3.8370000000000001E-3</v>
+        <v>2.8465000000000001E-3</v>
       </c>
       <c r="F60">
-        <v>1.8069999999999999E-2</v>
+        <v>1.0792E-2</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="C61">
-        <v>4.26E-4</v>
+        <v>3.3700000000000001E-4</v>
       </c>
       <c r="D61">
-        <v>1.188E-3</v>
+        <v>9.8900000000000008E-4</v>
       </c>
       <c r="E61">
-        <v>4.0029999999999996E-3</v>
+        <v>3.0240000000000002E-3</v>
       </c>
       <c r="F61">
-        <v>1.8110000000000001E-2</v>
+        <v>1.1409000000000001E-2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="C62">
-        <v>2.6200000000000003E-4</v>
+        <v>2.2599999999999999E-4</v>
       </c>
       <c r="D62">
-        <v>9.5299999999999996E-4</v>
+        <v>8.5700000000000001E-4</v>
       </c>
       <c r="E62">
-        <v>4.2750000000000002E-3</v>
+        <v>3.2179999999999999E-3</v>
       </c>
       <c r="F62">
-        <v>1.8179000000000001E-2</v>
+        <v>1.1612000000000001E-2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="C63">
-        <v>2.1699999999999999E-4</v>
+        <v>3.79E-4</v>
       </c>
       <c r="D63">
-        <v>9.0700000000000004E-4</v>
+        <v>1.0399999999999999E-3</v>
       </c>
       <c r="E63">
-        <v>4.1460000000000004E-3</v>
+        <v>3.5040000000000002E-3</v>
       </c>
       <c r="F63">
-        <v>1.8234E-2</v>
+        <v>1.1759E-2</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C64">
-        <v>2.4399999999999999E-4</v>
+        <v>3.6299999999999999E-4</v>
       </c>
       <c r="D64">
-        <v>1.0610000000000001E-3</v>
+        <v>1.15E-3</v>
       </c>
       <c r="E64">
-        <v>4.6540000000000002E-3</v>
+        <v>3.2030000000000001E-3</v>
       </c>
       <c r="F64">
-        <v>1.8636E-2</v>
+        <v>1.1877E-2</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="C65">
-        <v>2.8800000000000001E-4</v>
+        <v>3.6900000000000002E-4</v>
       </c>
       <c r="D65">
-        <v>1.1460000000000001E-3</v>
+        <v>1.4989999999999999E-3</v>
       </c>
       <c r="E65">
-        <v>4.6820000000000004E-3</v>
+        <v>3.6830000000000001E-3</v>
       </c>
       <c r="F65">
-        <v>1.8748999999999998E-2</v>
+        <v>1.2311000000000001E-2</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2011,259 +2011,259 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C66">
-        <v>3.21E-4</v>
+        <v>2.31E-4</v>
       </c>
       <c r="D66">
-        <v>1.07E-3</v>
+        <v>9.41E-4</v>
       </c>
       <c r="E66">
-        <v>4.4380000000000001E-3</v>
+        <v>2.5690000000000001E-3</v>
       </c>
       <c r="F66">
-        <v>1.8865E-2</v>
+        <v>1.3143E-2</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C67">
-        <v>2.7399999999999999E-4</v>
+        <v>4.0499999999999998E-4</v>
       </c>
       <c r="D67">
-        <v>1.077E-3</v>
+        <v>9.7099999999999997E-4</v>
       </c>
       <c r="E67">
-        <v>4.5100000000000001E-3</v>
+        <v>3.473E-3</v>
       </c>
       <c r="F67">
-        <v>1.9091E-2</v>
+        <v>1.4128E-2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="C68">
-        <v>2.7999999999999998E-4</v>
+        <v>4.4749999999999998E-4</v>
       </c>
       <c r="D68">
-        <v>1.023E-3</v>
+        <v>1.3324999999999999E-3</v>
       </c>
       <c r="E68">
-        <v>4.3489999999999996E-3</v>
+        <v>4.28E-3</v>
       </c>
       <c r="F68">
-        <v>1.9205E-2</v>
+        <v>1.5374000000000001E-2</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C69">
-        <v>3.19E-4</v>
+        <v>3.5100000000000002E-4</v>
       </c>
       <c r="D69">
-        <v>1.2099999999999999E-3</v>
+        <v>9.7599999999999998E-4</v>
       </c>
       <c r="E69">
-        <v>4.6680000000000003E-3</v>
+        <v>3.6240000000000001E-3</v>
       </c>
       <c r="F69">
-        <v>1.9258999999999998E-2</v>
+        <v>1.7665E-2</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C70">
-        <v>4.6099999999999998E-4</v>
+        <v>3.21E-4</v>
       </c>
       <c r="D70">
-        <v>1.4189999999999999E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="E70">
-        <v>4.9179999999999996E-3</v>
+        <v>4.4380000000000001E-3</v>
       </c>
       <c r="F70">
-        <v>2.0695000000000002E-2</v>
+        <v>1.8865E-2</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C71">
-        <v>4.9649999999999998E-4</v>
+        <v>4.7699999999999999E-4</v>
       </c>
       <c r="D71">
-        <v>1.4265E-3</v>
+        <v>1.611E-3</v>
       </c>
       <c r="E71">
-        <v>4.9754999999999999E-3</v>
+        <v>6.0920000000000002E-3</v>
       </c>
       <c r="F71">
-        <v>2.0997999999999999E-2</v>
+        <v>3.1171999999999998E-2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C72">
-        <v>5.1749999999999995E-4</v>
+        <v>3.8299999999999999E-4</v>
       </c>
       <c r="D72">
-        <v>1.4235000000000001E-3</v>
+        <v>1.6310000000000001E-3</v>
       </c>
       <c r="E72">
-        <v>5.2325000000000002E-3</v>
+        <v>7.2639999999999996E-3</v>
       </c>
       <c r="F72">
-        <v>2.17755E-2</v>
+        <v>3.7185000000000003E-2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C73">
-        <v>4.5199999999999998E-4</v>
+        <v>4.2400000000000001E-4</v>
       </c>
       <c r="D73">
-        <v>1.379E-3</v>
+        <v>1.503E-3</v>
       </c>
       <c r="E73">
-        <v>5.1905000000000007E-3</v>
+        <v>7.2519999999999998E-3</v>
       </c>
       <c r="F73">
-        <v>2.1794999999999998E-2</v>
+        <v>3.9962999999999999E-2</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C74">
-        <v>3.4699999999999998E-4</v>
+        <v>5.9000000000000003E-4</v>
       </c>
       <c r="D74">
-        <v>1.3359999999999999E-3</v>
+        <v>2.1064999999999999E-3</v>
       </c>
       <c r="E74">
-        <v>4.9909999999999998E-3</v>
+        <v>1.1309E-2</v>
       </c>
       <c r="F74">
-        <v>2.2544000000000002E-2</v>
+        <v>7.0706500000000005E-2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B75" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="C75">
-        <v>3.9199999999999999E-4</v>
+        <v>2.6699999999999998E-4</v>
       </c>
       <c r="D75">
-        <v>1.3849999999999999E-3</v>
+        <v>7.0200000000000004E-4</v>
       </c>
       <c r="E75">
-        <v>5.2180000000000004E-3</v>
+        <v>2.8679999999999999E-3</v>
       </c>
       <c r="F75">
-        <v>2.3460999999999999E-2</v>
+        <v>3.3730000000000001E-3</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C76">
-        <v>3.8699999999999997E-4</v>
+        <v>4.0299999999999998E-4</v>
       </c>
       <c r="D76">
-        <v>1.5319999999999999E-3</v>
+        <v>1.3090000000000001E-3</v>
       </c>
       <c r="E76">
-        <v>6.1859999999999997E-3</v>
+        <v>2.931E-3</v>
       </c>
       <c r="F76">
-        <v>3.0535E-2</v>
+        <v>7.816E-3</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="C77">
-        <v>4.7699999999999999E-4</v>
+        <v>3.4600000000000001E-4</v>
       </c>
       <c r="D77">
-        <v>1.611E-3</v>
+        <v>1.116E-3</v>
       </c>
       <c r="E77">
-        <v>6.0920000000000002E-3</v>
+        <v>2.9020000000000001E-3</v>
       </c>
       <c r="F77">
-        <v>3.1171999999999998E-2</v>
+        <v>7.9900000000000006E-3</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B78" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C78">
-        <v>3.8299999999999999E-4</v>
+        <v>3.1799999999999998E-4</v>
       </c>
       <c r="D78">
-        <v>1.6310000000000001E-3</v>
+        <v>8.5400000000000005E-4</v>
       </c>
       <c r="E78">
-        <v>7.2639999999999996E-3</v>
+        <v>2.5070000000000001E-3</v>
       </c>
       <c r="F78">
-        <v>3.7185000000000003E-2</v>
+        <v>8.6029999999999995E-3</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2271,385 +2271,385 @@
         <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C79">
-        <v>4.2000000000000002E-4</v>
+        <v>4.26E-4</v>
       </c>
       <c r="D79">
-        <v>1.658E-3</v>
+        <v>1.0560000000000001E-3</v>
       </c>
       <c r="E79">
-        <v>7.613E-3</v>
+        <v>2.8530000000000001E-3</v>
       </c>
       <c r="F79">
-        <v>3.7642000000000002E-2</v>
+        <v>1.07435E-2</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="C80">
-        <v>3.7399999999999998E-4</v>
+        <v>3.8099999999999999E-4</v>
       </c>
       <c r="D80">
-        <v>1.5269999999999999E-3</v>
+        <v>1.052E-3</v>
       </c>
       <c r="E80">
-        <v>7.9869999999999993E-3</v>
+        <v>3.2699999999999999E-3</v>
       </c>
       <c r="F80">
-        <v>3.9775999999999999E-2</v>
+        <v>1.0926E-2</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="C81">
-        <v>4.2400000000000001E-4</v>
+        <v>2.8600000000000001E-4</v>
       </c>
       <c r="D81">
-        <v>1.503E-3</v>
+        <v>9.2299999999999999E-4</v>
       </c>
       <c r="E81">
-        <v>7.2519999999999998E-3</v>
+        <v>3.0040000000000002E-3</v>
       </c>
       <c r="F81">
-        <v>3.9962999999999999E-2</v>
+        <v>1.149E-2</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B82" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C82">
-        <v>9.3749999999999997E-4</v>
+        <v>2.6600000000000001E-4</v>
       </c>
       <c r="D82">
-        <v>1.7485000000000001E-3</v>
+        <v>9.0499999999999999E-4</v>
       </c>
       <c r="E82">
-        <v>9.5079999999999991E-3</v>
+        <v>3.212E-3</v>
       </c>
       <c r="F82">
-        <v>6.8498000000000003E-2</v>
+        <v>1.1629E-2</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="C83">
-        <v>1.1225E-3</v>
+        <v>3.9300000000000001E-4</v>
       </c>
       <c r="D83">
-        <v>1.7930000000000001E-3</v>
+        <v>1.1980000000000001E-3</v>
       </c>
       <c r="E83">
-        <v>9.3880000000000005E-3</v>
+        <v>3.2780000000000001E-3</v>
       </c>
       <c r="F83">
-        <v>6.8598999999999993E-2</v>
+        <v>1.1771E-2</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C84">
-        <v>5.1350000000000007E-4</v>
+        <v>4.1199999999999999E-4</v>
       </c>
       <c r="D84">
-        <v>2.006E-3</v>
+        <v>1.1360000000000001E-3</v>
       </c>
       <c r="E84">
-        <v>1.1375E-2</v>
+        <v>3.5720000000000001E-3</v>
       </c>
       <c r="F84">
-        <v>6.9242999999999999E-2</v>
+        <v>1.2093E-2</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C85">
-        <v>5.8399999999999999E-4</v>
+        <v>3.5799999999999997E-4</v>
       </c>
       <c r="D85">
-        <v>2.0704999999999999E-3</v>
+        <v>1.0349999999999999E-3</v>
       </c>
       <c r="E85">
-        <v>1.14365E-2</v>
+        <v>2.4229999999999998E-3</v>
       </c>
       <c r="F85">
-        <v>6.9770499999999999E-2</v>
+        <v>1.2233000000000001E-2</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="C86">
-        <v>5.9000000000000003E-4</v>
+        <v>2.7900000000000001E-4</v>
       </c>
       <c r="D86">
-        <v>2.1064999999999999E-3</v>
+        <v>1.0200000000000001E-3</v>
       </c>
       <c r="E86">
-        <v>1.1309E-2</v>
+        <v>2.65E-3</v>
       </c>
       <c r="F86">
-        <v>7.0706500000000005E-2</v>
+        <v>1.3396999999999999E-2</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="C87">
-        <v>5.3000000000000009E-4</v>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="D87">
-        <v>2.0045000000000002E-3</v>
+        <v>8.2299999999999995E-4</v>
       </c>
       <c r="E87">
-        <v>1.1518499999999999E-2</v>
+        <v>3.1480000000000002E-3</v>
       </c>
       <c r="F87">
-        <v>7.0735500000000007E-2</v>
+        <v>1.3505E-2</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B88" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="C88">
-        <v>4.5600000000000003E-4</v>
+        <v>3.79E-4</v>
       </c>
       <c r="D88">
-        <v>2.2285E-3</v>
+        <v>9.8799999999999995E-4</v>
       </c>
       <c r="E88">
-        <v>1.392E-2</v>
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="F88">
-        <v>8.5014499999999993E-2</v>
+        <v>1.7812000000000001E-2</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="C89">
-        <v>4.46E-4</v>
+        <v>3.57E-4</v>
       </c>
       <c r="D89">
-        <v>2.0225E-3</v>
+        <v>1.085E-3</v>
       </c>
       <c r="E89">
-        <v>1.3827000000000001E-2</v>
+        <v>3.8370000000000001E-3</v>
       </c>
       <c r="F89">
-        <v>9.0217999999999993E-2</v>
+        <v>1.8069999999999999E-2</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B90" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="C90">
-        <v>5.0850000000000005E-4</v>
+        <v>4.2000000000000002E-4</v>
       </c>
       <c r="D90">
-        <v>2.1105E-3</v>
+        <v>1.658E-3</v>
       </c>
       <c r="E90">
-        <v>1.4120000000000001E-2</v>
+        <v>7.613E-3</v>
       </c>
       <c r="F90">
-        <v>9.1477500000000003E-2</v>
+        <v>3.7642000000000002E-2</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="C91">
-        <v>5.7649999999999997E-4</v>
+        <v>3.9899999999999999E-4</v>
       </c>
       <c r="D91">
-        <v>2.1580000000000002E-3</v>
+        <v>1.201E-3</v>
       </c>
       <c r="E91">
-        <v>1.3648E-2</v>
+        <v>3.1749999999999999E-3</v>
       </c>
       <c r="F91">
-        <v>9.7140499999999991E-2</v>
+        <v>8.8240000000000002E-3</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="C92">
-        <v>7.5700000000000008E-4</v>
+        <v>3.2400000000000001E-4</v>
       </c>
       <c r="D92">
-        <v>2.3995000000000002E-3</v>
+        <v>9.5699999999999995E-4</v>
       </c>
       <c r="E92">
-        <v>1.074E-2</v>
+        <v>3.0839999999999999E-3</v>
       </c>
       <c r="F92">
-        <v>9.7824500000000009E-2</v>
+        <v>1.1233999999999999E-2</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B93" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="C93">
-        <v>6.4400000000000004E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="D93">
-        <v>2.493E-3</v>
+        <v>1.142E-3</v>
       </c>
       <c r="E93">
-        <v>1.1592E-2</v>
+        <v>2.421E-3</v>
       </c>
       <c r="F93">
-        <v>9.8580500000000001E-2</v>
+        <v>1.2428E-2</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="C94">
-        <v>1.0839999999999999E-3</v>
+        <v>2.9100000000000003E-4</v>
       </c>
       <c r="D94">
-        <v>2.4784999999999998E-3</v>
+        <v>1.157E-3</v>
       </c>
       <c r="E94">
-        <v>1.50565E-2</v>
+        <v>3.718E-3</v>
       </c>
       <c r="F94">
-        <v>0.100032</v>
+        <v>1.3157E-2</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="C95">
-        <v>1.2784999999999999E-3</v>
+        <v>2.7599999999999999E-4</v>
       </c>
       <c r="D95">
-        <v>2.5214999999999999E-3</v>
+        <v>8.9099999999999997E-4</v>
       </c>
       <c r="E95">
-        <v>1.5318999999999999E-2</v>
+        <v>3.2330000000000002E-3</v>
       </c>
       <c r="F95">
-        <v>0.1004125</v>
+        <v>1.3602E-2</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="C96">
-        <v>9.5549999999999997E-4</v>
+        <v>4.26E-4</v>
       </c>
       <c r="D96">
-        <v>2.5665000000000002E-3</v>
+        <v>1.188E-3</v>
       </c>
       <c r="E96">
-        <v>1.6927500000000002E-2</v>
+        <v>4.0029999999999996E-3</v>
       </c>
       <c r="F96">
-        <v>0.11158949999999999</v>
+        <v>1.8110000000000001E-2</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B97" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="C97">
-        <v>1.1410000000000001E-3</v>
+        <v>3.9599999999999998E-4</v>
       </c>
       <c r="D97">
-        <v>2.6424999999999999E-3</v>
+        <v>1.209E-3</v>
       </c>
       <c r="E97">
-        <v>1.7187999999999998E-2</v>
+        <v>3.803E-3</v>
       </c>
       <c r="F97">
-        <v>0.1120165</v>
+        <v>1.3332E-2</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F97" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F97">
-      <sortCondition ref="F1:F97"/>
+      <sortCondition ref="A1:A97"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>